<commit_message>
Sheet Updated Till 30th Jan 2024
</commit_message>
<xml_diff>
--- a/DSA Status.xlsx
+++ b/DSA Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DSA Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B7DD8A-ED44-4A6F-AABC-7F7AF3196DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9256CC84-C7E1-4F74-A966-FEECA76D654D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Sl No</t>
   </si>
@@ -64,6 +64,42 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-sorted-array/description/?envType=study-plan-v2&amp;envId=top-interview-150</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Leetcode Top Interview 150</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>Remove Element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-element/description/?envType=study-plan-v2&amp;envId=top-interview-150</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-duplicates-from-sorted-array/description/?envType=study-plan-v2&amp;envId=top-interview-150</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/majority-element/description/?envType=study-plan-v2&amp;envId=top-interview-150</t>
+  </si>
+  <si>
+    <t>Majority Element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle/description/?envType=study-plan-v2&amp;envId=top-interview-150</t>
+  </si>
+  <si>
+    <t>Linked List Cycle</t>
   </si>
 </sst>
 </file>
@@ -94,7 +130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +140,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,11 +178,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -422,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,9 +528,114 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://leetcode.com/problems/frequency-of-the-most-frequent-element/" xr:uid="{A81FE196-AE9D-4A0E-A4BB-06AA689D99EF}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://leetcode.com/problems/merge-sorted-array/" xr:uid="{79C77D50-B07A-459E-BE0F-7A800F87C372}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://leetcode.com/problems/remove-element/" xr:uid="{C68FEC88-FC07-441D-86A5-8A84005DB336}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array/" xr:uid="{A5803B89-3511-4436-A236-4D34463ACB11}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://leetcode.com/problems/majority-element/" xr:uid="{013BAA69-BE70-42E9-8DF2-09909520B1AD}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://leetcode.com/problems/linked-list-cycle/" xr:uid="{6C78BBFB-B008-4B71-BCF9-A482E4339470}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>